<commit_message>
Update 2020-03-23 19:10 East Timor works
</commit_message>
<xml_diff>
--- a/COVID-19 Apps/Population Data.xlsx
+++ b/COVID-19 Apps/Population Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zur Bonsen Georg\Documents\Programme\Beyond4P_Apps\COVID-19 Apps\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AE84800-62D0-4FF3-BA35-64DBC95D983C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{307D929A-7204-419D-8BCA-68B8E0DD9412}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15960" xr2:uid="{F1D96CA6-85D8-47A9-B3B5-9350C0EB077E}"/>
   </bookViews>
@@ -3131,6 +3131,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -3162,7 +3163,6 @@
     <xf numFmtId="0" fontId="5" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Link" xfId="1" builtinId="8"/>
@@ -3481,8 +3481,8 @@
   <dimension ref="A1:K376"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A344" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B367" sqref="B367"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14105,7 +14105,7 @@
       <c r="B355" s="97" t="s">
         <v>751</v>
       </c>
-      <c r="C355" s="113" t="s">
+      <c r="C355" s="102" t="s">
         <v>772</v>
       </c>
       <c r="D355" s="97"/>
@@ -14525,13 +14525,13 @@
       <c r="C6" s="53" t="s">
         <v>662</v>
       </c>
-      <c r="D6" s="104" t="s">
+      <c r="D6" s="105" t="s">
         <v>664</v>
       </c>
-      <c r="E6" s="102" t="s">
+      <c r="E6" s="103" t="s">
         <v>3</v>
       </c>
-      <c r="F6" s="103"/>
+      <c r="F6" s="104"/>
       <c r="G6" s="53" t="s">
         <v>666</v>
       </c>
@@ -14541,14 +14541,14 @@
       <c r="I6" s="53" t="s">
         <v>3</v>
       </c>
-      <c r="J6" s="104" t="s">
+      <c r="J6" s="105" t="s">
         <v>672</v>
       </c>
-      <c r="K6" s="104"/>
-      <c r="L6" s="102" t="s">
+      <c r="K6" s="105"/>
+      <c r="L6" s="103" t="s">
         <v>674</v>
       </c>
-      <c r="M6" s="103"/>
+      <c r="M6" s="104"/>
       <c r="N6" s="53" t="s">
         <v>666</v>
       </c>
@@ -14557,11 +14557,11 @@
       <c r="C7" s="57" t="s">
         <v>663</v>
       </c>
-      <c r="D7" s="104"/>
-      <c r="E7" s="104" t="s">
+      <c r="D7" s="105"/>
+      <c r="E7" s="105" t="s">
         <v>665</v>
       </c>
-      <c r="F7" s="104"/>
+      <c r="F7" s="105"/>
       <c r="G7" s="57" t="s">
         <v>667</v>
       </c>
@@ -14571,21 +14571,21 @@
       <c r="I7" s="57" t="s">
         <v>670</v>
       </c>
-      <c r="J7" s="104" t="s">
+      <c r="J7" s="105" t="s">
         <v>673</v>
       </c>
-      <c r="K7" s="104"/>
-      <c r="L7" s="104" t="s">
+      <c r="K7" s="105"/>
+      <c r="L7" s="105" t="s">
         <v>675</v>
       </c>
-      <c r="M7" s="104"/>
+      <c r="M7" s="105"/>
       <c r="N7" s="57" t="s">
         <v>676</v>
       </c>
     </row>
     <row r="8" spans="3:14" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C8" s="54"/>
-      <c r="D8" s="104"/>
+      <c r="D8" s="105"/>
       <c r="E8" s="59" t="s">
         <v>677</v>
       </c>
@@ -15369,10 +15369,10 @@
       </c>
     </row>
     <row r="2" spans="1:12" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="105" t="s">
+      <c r="A2" s="106" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="105" t="s">
+      <c r="B2" s="106" t="s">
         <v>2</v>
       </c>
       <c r="C2" s="11" t="s">
@@ -15407,8 +15407,8 @@
       </c>
     </row>
     <row r="3" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="106"/>
-      <c r="B3" s="106"/>
+      <c r="A3" s="107"/>
+      <c r="B3" s="107"/>
       <c r="C3" s="2">
         <v>-2020</v>
       </c>
@@ -24613,7 +24613,7 @@
       <c r="D1" t="s">
         <v>405</v>
       </c>
-      <c r="I1" s="107" t="s">
+      <c r="I1" s="108" t="s">
         <v>232</v>
       </c>
       <c r="J1" s="83"/>
@@ -24632,7 +24632,7 @@
         <f t="shared" ref="D2:D33" si="0">"US " &amp;A2</f>
         <v>US Alabama</v>
       </c>
-      <c r="I2" s="108"/>
+      <c r="I2" s="109"/>
       <c r="J2" s="59" t="s">
         <v>696</v>
       </c>
@@ -25566,46 +25566,46 @@
   <sheetData>
     <row r="4" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="5" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B5" s="111" t="s">
+      <c r="B5" s="112" t="s">
         <v>409</v>
       </c>
-      <c r="C5" s="111" t="s">
+      <c r="C5" s="112" t="s">
         <v>410</v>
       </c>
-      <c r="D5" s="107" t="s">
+      <c r="D5" s="108" t="s">
         <v>411</v>
       </c>
       <c r="E5" s="23" t="s">
         <v>412</v>
       </c>
-      <c r="F5" s="107" t="s">
+      <c r="F5" s="108" t="s">
         <v>414</v>
       </c>
-      <c r="G5" s="109" t="s">
+      <c r="G5" s="110" t="s">
         <v>415</v>
       </c>
-      <c r="H5" s="109" t="s">
+      <c r="H5" s="110" t="s">
         <v>416</v>
       </c>
-      <c r="I5" s="109" t="s">
+      <c r="I5" s="110" t="s">
         <v>417</v>
       </c>
-      <c r="J5" s="109" t="s">
+      <c r="J5" s="110" t="s">
         <v>418</v>
       </c>
     </row>
     <row r="6" spans="2:11" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="112"/>
-      <c r="C6" s="112"/>
-      <c r="D6" s="108"/>
+      <c r="B6" s="113"/>
+      <c r="C6" s="113"/>
+      <c r="D6" s="109"/>
       <c r="E6" s="24" t="s">
         <v>413</v>
       </c>
-      <c r="F6" s="108"/>
-      <c r="G6" s="110"/>
-      <c r="H6" s="110"/>
-      <c r="I6" s="110"/>
-      <c r="J6" s="110"/>
+      <c r="F6" s="109"/>
+      <c r="G6" s="111"/>
+      <c r="H6" s="111"/>
+      <c r="I6" s="111"/>
+      <c r="J6" s="111"/>
     </row>
     <row r="7" spans="2:11" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="25" t="s">

</xml_diff>